<commit_message>
[BE-Edit] Finalize import template
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_coa.xlsx
+++ b/budgetin/api/utils/template/import_template_coa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U071182\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U071182\Documents\04. BIT\Budgetin\Budgetin\budgetin\api\utils\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="coa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>coa_name</t>
   </si>
@@ -45,42 +45,6 @@
     <t>Biaya Pengelola Pendukung Proses</t>
   </si>
   <si>
-    <t>Consultant</t>
-  </si>
-  <si>
-    <t>Gedung</t>
-  </si>
-  <si>
-    <t>HW</t>
-  </si>
-  <si>
-    <t>Keperluan Kantor Lainnya</t>
-  </si>
-  <si>
-    <t>Keperluan Komputer</t>
-  </si>
-  <si>
-    <t>M. HW</t>
-  </si>
-  <si>
-    <t>M. SW</t>
-  </si>
-  <si>
-    <t>Pemanfaatan IT</t>
-  </si>
-  <si>
-    <t>Pemeliharaan Gedung &amp; Perabotan</t>
-  </si>
-  <si>
-    <t>Promosi</t>
-  </si>
-  <si>
-    <t>Sewa Gedung</t>
-  </si>
-  <si>
-    <t>SW</t>
-  </si>
-  <si>
     <t>COA untuk ASET ROA TANAH</t>
   </si>
   <si>
@@ -97,78 +61,6 @@
   </si>
   <si>
     <t>Hyperion Biaya Pengelola Pendukung Proses</t>
-  </si>
-  <si>
-    <t>COA untuk Consultant</t>
-  </si>
-  <si>
-    <t>Hyperion Consultant</t>
-  </si>
-  <si>
-    <t>COA untuk Gedung</t>
-  </si>
-  <si>
-    <t>Hyperion Gedung</t>
-  </si>
-  <si>
-    <t>COA untuk HW</t>
-  </si>
-  <si>
-    <t>Hyperion HW</t>
-  </si>
-  <si>
-    <t>COA untuk Keperluan Kantor Lainnya</t>
-  </si>
-  <si>
-    <t>Hyperion Keperluan Kantor Lainnya</t>
-  </si>
-  <si>
-    <t>COA untuk Keperluan Komputer</t>
-  </si>
-  <si>
-    <t>Hyperion Keperluan Komputer</t>
-  </si>
-  <si>
-    <t>COA untuk M. HW</t>
-  </si>
-  <si>
-    <t>Hyperion M. HW</t>
-  </si>
-  <si>
-    <t>COA untuk M. SW</t>
-  </si>
-  <si>
-    <t>Hyperion M. SW</t>
-  </si>
-  <si>
-    <t>COA untuk Pemanfaatan IT</t>
-  </si>
-  <si>
-    <t>Hyperion Pemanfaatan IT</t>
-  </si>
-  <si>
-    <t>COA untuk Pemeliharaan Gedung &amp; Perabotan</t>
-  </si>
-  <si>
-    <t>Hyperion Pemeliharaan Gedung &amp; Perabotan</t>
-  </si>
-  <si>
-    <t>COA untuk Promosi</t>
-  </si>
-  <si>
-    <t>Hyperion Promosi</t>
-  </si>
-  <si>
-    <t>COA untuk Sewa Gedung</t>
-  </si>
-  <si>
-    <t>Hyperion Sewa Gedung</t>
-  </si>
-  <si>
-    <t>COA untuk SW</t>
-  </si>
-  <si>
-    <t>Hyperion SW</t>
   </si>
 </sst>
 </file>
@@ -486,20 +378,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,171 +400,6 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -688,14 +415,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,37 +433,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>